<commit_message>
AJUSTE ADIÇÃO DO CÓDIGO DO PRODUTO VISUALIZAR ITENS BOLSA SAIDA AO SELECIONAR O RESUMO
</commit_message>
<xml_diff>
--- a/Almoxarifado/Modelos/RECIBO_SAIDA.xlsx
+++ b/Almoxarifado/Modelos/RECIBO_SAIDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIPOLATTI\SISTEMAS\Almoxarifado\Almoxarifado\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BD0708-DEEA-43C3-83CC-20697EF1AF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D27E749-42A0-4A3B-820E-5D7297960316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{6AA88C75-C6FE-45C6-A43E-D44C06A268E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{6AA88C75-C6FE-45C6-A43E-D44C06A268E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>CIPOLATTI E CIPOLATTI LOCAÇÃO E COMÉRCIO LTDA</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>TOTAL DA BOLSA:</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -195,6 +198,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -204,20 +213,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -555,183 +558,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEF6767-C6F4-4506-800F-B698A8BFEFC3}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:H10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="1" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="4"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
       <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="9" t="s">
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="4">
-        <f>SUM(K7:K8)</f>
+      <c r="K9" s="11"/>
+      <c r="L9" s="4">
+        <f>SUM(L7:L8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K4"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="J9:K9"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.31496062992125984" bottom="0.31496062992125984" header="0.15748031496062992" footer="0.15748031496062992"/>
-  <pageSetup paperSize="9" scale="96" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="88" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;L &amp;D &amp;T&amp;R&amp;P de &amp;N                </oddFooter>
   </headerFooter>

</xml_diff>